<commit_message>
Latest version of the randomization for the fall planted expt, Sept 2023
</commit_message>
<xml_diff>
--- a/data/UON24_Entries.xlsx
+++ b/data/UON24_Entries.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jj332/Documents/GitRepo/IntercroppingOatPea/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E8E3FA61-27DD-4946-B077-4174D3A08A19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B06E5B0-E8F1-E347-969A-65DE188C2A7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="29040" windowHeight="15840" xr2:uid="{98299EA3-8724-43D4-A725-9BB46D7157F5}"/>
   </bookViews>
@@ -153,7 +153,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="85">
   <si>
     <t>EXPT</t>
   </si>
@@ -441,6 +441,9 @@
       </rPr>
       <t>) 2023-2024</t>
     </r>
+  </si>
+  <si>
+    <t>Drop from NY (first five based on pedigree after that ??)</t>
   </si>
 </sst>
 </file>
@@ -23384,11 +23387,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{282FDCBE-8418-4550-9952-6A15A7EA999D}">
-  <dimension ref="A1:G36"/>
+  <dimension ref="A1:H36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E21" sqref="E21"/>
+      <selection pane="bottomLeft" activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
@@ -23844,7 +23847,7 @@
     <col min="16117" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="43" t="s">
         <v>83</v>
       </c>
@@ -23855,7 +23858,7 @@
       <c r="F1" s="44"/>
       <c r="G1" s="45"/>
     </row>
-    <row r="2" spans="1:7" s="7" customFormat="1" ht="76.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" s="7" customFormat="1" ht="76.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -23877,8 +23880,11 @@
       <c r="G2" s="6" t="s">
         <v>6</v>
       </c>
+      <c r="H2" s="7" t="s">
+        <v>84</v>
+      </c>
     </row>
-    <row r="3" spans="1:7" s="14" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:8" s="14" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A3" s="8" t="s">
         <v>7</v>
       </c>
@@ -23901,7 +23907,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="14" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:8" s="14" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A4" s="15" t="s">
         <v>7</v>
       </c>
@@ -23924,7 +23930,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="14" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:8" s="14" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A5" s="15" t="s">
         <v>7</v>
       </c>
@@ -23947,7 +23953,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="14" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:8" s="14" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A6" s="15" t="s">
         <v>7</v>
       </c>
@@ -23970,7 +23976,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="14" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:8" s="14" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A7" s="15" t="s">
         <v>7</v>
       </c>
@@ -23993,7 +23999,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="14" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:8" s="14" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A8" s="23" t="s">
         <v>7</v>
       </c>
@@ -24016,7 +24022,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="14" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:8" s="14" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A9" s="23" t="s">
         <v>7</v>
       </c>
@@ -24039,7 +24045,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:8" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="23" t="s">
         <v>7</v>
       </c>
@@ -24062,7 +24068,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:7" s="14" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:8" s="14" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A11" s="23" t="s">
         <v>7</v>
       </c>
@@ -24085,7 +24091,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="14" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:8" s="14" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A12" s="23" t="s">
         <v>7</v>
       </c>
@@ -24108,7 +24114,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="14" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:8" s="14" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A13" s="23" t="s">
         <v>7</v>
       </c>
@@ -24131,7 +24137,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="14" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:8" s="14" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A14" s="15" t="s">
         <v>7</v>
       </c>
@@ -24154,7 +24160,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:7" s="14" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:8" s="14" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A15" s="15" t="s">
         <v>7</v>
       </c>
@@ -24177,7 +24183,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:7" s="14" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:8" s="14" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A16" s="15" t="s">
         <v>7</v>
       </c>
@@ -24199,8 +24205,11 @@
       <c r="G16" s="20" t="s">
         <v>26</v>
       </c>
+      <c r="H16" s="14">
+        <v>8</v>
+      </c>
     </row>
-    <row r="17" spans="1:7" s="14" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:8" s="14" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A17" s="15" t="s">
         <v>7</v>
       </c>
@@ -24223,7 +24232,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:7" s="14" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:8" s="14" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A18" s="15" t="s">
         <v>7</v>
       </c>
@@ -24246,7 +24255,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:7" s="14" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:8" s="14" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A19" s="15" t="s">
         <v>7</v>
       </c>
@@ -24268,8 +24277,11 @@
       <c r="G19" s="20" t="s">
         <v>26</v>
       </c>
+      <c r="H19" s="14">
+        <v>1</v>
+      </c>
     </row>
-    <row r="20" spans="1:7" s="14" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:8" s="14" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A20" s="15" t="s">
         <v>7</v>
       </c>
@@ -24292,7 +24304,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="21" spans="1:7" s="14" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:8" s="14" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A21" s="23" t="s">
         <v>7</v>
       </c>
@@ -24315,7 +24327,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="1:7" s="14" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:8" s="14" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A22" s="23" t="s">
         <v>7</v>
       </c>
@@ -24338,7 +24350,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:7" s="14" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:8" s="14" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A23" s="23" t="s">
         <v>7</v>
       </c>
@@ -24361,7 +24373,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="1:7" s="14" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:8" s="14" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A24" s="15" t="s">
         <v>7</v>
       </c>
@@ -24384,7 +24396,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="25" spans="1:7" s="14" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:8" s="14" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A25" s="15" t="s">
         <v>7</v>
       </c>
@@ -24407,7 +24419,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="1:7" s="14" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:8" s="14" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A26" s="15" t="s">
         <v>7</v>
       </c>
@@ -24429,8 +24441,11 @@
       <c r="G26" s="20" t="s">
         <v>26</v>
       </c>
+      <c r="H26" s="14">
+        <v>2</v>
+      </c>
     </row>
-    <row r="27" spans="1:7" s="14" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:8" s="14" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A27" s="15" t="s">
         <v>7</v>
       </c>
@@ -24452,8 +24467,11 @@
       <c r="G27" s="20" t="s">
         <v>26</v>
       </c>
+      <c r="H27" s="14">
+        <v>3</v>
+      </c>
     </row>
-    <row r="28" spans="1:7" s="14" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:8" s="14" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A28" s="15" t="s">
         <v>7</v>
       </c>
@@ -24476,7 +24494,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:7" s="14" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:8" s="14" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A29" s="15" t="s">
         <v>7</v>
       </c>
@@ -24498,8 +24516,11 @@
       <c r="G29" s="20" t="s">
         <v>26</v>
       </c>
+      <c r="H29" s="14">
+        <v>4</v>
+      </c>
     </row>
-    <row r="30" spans="1:7" s="14" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:8" s="14" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A30" s="15" t="s">
         <v>7</v>
       </c>
@@ -24522,7 +24543,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="31" spans="1:7" s="14" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:8" s="14" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A31" s="15" t="s">
         <v>7</v>
       </c>
@@ -24544,8 +24565,11 @@
       <c r="G31" s="20" t="s">
         <v>26</v>
       </c>
+      <c r="H31" s="14">
+        <v>6</v>
+      </c>
     </row>
-    <row r="32" spans="1:7" s="14" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:8" s="14" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A32" s="23" t="s">
         <v>7</v>
       </c>
@@ -24568,7 +24592,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="33" spans="1:7" s="14" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:8" s="14" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A33" s="23" t="s">
         <v>7</v>
       </c>
@@ -24590,8 +24614,11 @@
       <c r="G33" s="28" t="s">
         <v>26</v>
       </c>
+      <c r="H33" s="14">
+        <v>5</v>
+      </c>
     </row>
-    <row r="34" spans="1:7" s="14" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:8" s="14" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A34" s="23" t="s">
         <v>7</v>
       </c>
@@ -24614,7 +24641,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="35" spans="1:7" s="14" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:8" s="14" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A35" s="23" t="s">
         <v>7</v>
       </c>
@@ -24636,8 +24663,11 @@
       <c r="G35" s="28" t="s">
         <v>23</v>
       </c>
+      <c r="H35" s="14">
+        <v>7</v>
+      </c>
     </row>
-    <row r="36" spans="1:7" s="14" customFormat="1" ht="14" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:8" s="14" customFormat="1" ht="14" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A36" s="34" t="s">
         <v>7</v>
       </c>

</xml_diff>